<commit_message>
Sistemazione route classi e punti di raccolta
</commit_message>
<xml_diff>
--- a/runout/puntiraccolta.xlsx
+++ b/runout/puntiraccolta.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Punti Raccolta 2526" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Punti Raccolta 2526" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -41,13 +41,13 @@
 1-12</t>
   </si>
   <si>
-    <t>LAB DIS - 1</t>
-  </si>
-  <si>
-    <t>LAB LTO
-PALESTRA 1
-PALESTRA 2
-SALA PESI</t>
+    <t>1-32</t>
+  </si>
+  <si>
+    <t>LTO
+PAL1
+PAL2
+PALF</t>
   </si>
   <si>
     <t>1-14
@@ -60,7 +60,7 @@
 1-94
 1-95
 1-96
-BASKIN</t>
+PBAS</t>
   </si>
   <si>
     <t>PIANO TERRA
@@ -72,16 +72,28 @@
 M1-23</t>
   </si>
   <si>
-    <t>E1-7
+    <t>E0-1
+E0-2
+E0-3
+E1-7
 E1-8
+M0-1
+M0-2
+M0-3
 M1-8
 M1-11
 M1-18
+T0-1
 T1-6
 T1-7
 T1-12
 T1-13
 T1-14
+I0-1
+I0-2
+I0-3
+I0-4
+I0-5
 I1-1
 I1-2
 I1-3
@@ -98,7 +110,7 @@
 2-5
 2-6
 2-7
-LAB DIS - 2</t>
+2-8</t>
   </si>
   <si>
     <t>2-12</t>
@@ -552,6 +564,10 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>